<commit_message>
2nd committ yatra.com bus booking
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestCasesforBusBooking-Yatra.xlsx
+++ b/src/test/resources/testdata/TestCasesforBusBooking-Yatra.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16125" windowHeight="5880"/>
+    <workbookView windowWidth="15270" windowHeight="5880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,14 +104,15 @@
     <t>Select a Bus</t>
   </si>
   <si>
-    <t>1.select Bus Type
-2.Select Amenities
-3.Select No.of Passengers
-4.Sort by Duration
-5.Select any Bus as per requirements</t>
-  </si>
-  <si>
-    <t>Enter bus type and amenties.select no.of passengers and click sort by duration.select any bus.</t>
+    <t>1.Validating departfrom,goingto,deapartdate
+2.select Bus Type
+3.Select Amenities
+4.Select No.of Passengers
+5.Sort by Duration
+6.Select any Bus as per requirements</t>
+  </si>
+  <si>
+    <t>Validating the departfrom and to places, and validating date of journey.After clicking bus type and amenties.selecting no.of passengers and clicking sort by duration.select any bus.</t>
   </si>
   <si>
     <t xml:space="preserve">1.Enter Sleeper
@@ -129,9 +130,11 @@
     <t>Book a Bus</t>
   </si>
   <si>
-    <t>1.Select Bus Seats
-2.Choose Bording Point
-3.Click on Continue for signin to book a  bus</t>
+    <t>1.Validating Bus Type,Amenties
+2.Select Bus Seats
+3.Choose Bording Point
+4.Validating Bording Point,Bus Seats,Total Fare
+5.Click on Continue for signin to book a  bus</t>
   </si>
   <si>
     <t>After selecting bus.select any 3 seats and click continue button to goto next page.</t>
@@ -148,9 +151,10 @@
     <t>Signin to Book</t>
   </si>
   <si>
-    <t>1.Click emailaddress
-2.Click Phone Number
-3.Click BookAsGuest to fill travellers details</t>
+    <t>1.Validatite starting time and ending time
+2.Click emailaddress
+3.Click Phone Number
+4.Click BookAsGuest to fill travellers details</t>
   </si>
   <si>
     <t>After selecting bus seats enter emailid and phone number for confirmation.and click bookasguest for confirm the booking.</t>
@@ -175,8 +179,8 @@
     <t>fill all the passenger details like title,name and age of three passengers.and after entering details click continue for make payment.</t>
   </si>
   <si>
-    <t>1.Enter Mr,Bunny,20
-2.Enter Mr,Pavan,20
+    <t>1.Enter Mr,Bunny,18
+2.Enter Mr,Pavan,18
 3,Enter Ms,Anu,22</t>
   </si>
 </sst>
@@ -211,16 +215,99 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,6 +321,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -241,75 +337,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -318,24 +345,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,13 +354,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -364,19 +368,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,6 +416,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -400,151 +524,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -558,41 +562,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -616,16 +590,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -655,12 +635,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -678,130 +682,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1160,8 +1164,8 @@
   <sheetPr/>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1170,7 +1174,8 @@
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.2857142857143" style="1" customWidth="1"/>
-    <col min="5" max="6" width="39.1428571428571" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.2857142857143" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.8571428571429" style="2" customWidth="1"/>
     <col min="7" max="7" width="33.1428571428571" style="3" customWidth="1"/>
     <col min="8" max="8" width="19.5714285714286" style="1" customWidth="1"/>
   </cols>
@@ -1299,7 +1304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" ht="84" customHeight="1" spans="3:8">
+    <row r="9" ht="114" customHeight="1" spans="3:8">
       <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1319,7 +1324,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" ht="49" customHeight="1" spans="3:8">
+    <row r="10" ht="80" customHeight="1" spans="3:8">
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
@@ -1339,7 +1344,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" ht="66" customHeight="1" spans="3:8">
+    <row r="11" ht="81" customHeight="1" spans="3:8">
       <c r="C11" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>